<commit_message>
Mise à jour backend et OCR
</commit_message>
<xml_diff>
--- a/backend/templates/template_bordereau.xlsx
+++ b/backend/templates/template_bordereau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\ncosumar-main\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC58813E-4A18-4E93-97ED-E09969B25E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6C958-ED58-415D-B35E-74479AF50D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>N° Police</t>
   </si>
@@ -60,12 +60,15 @@
   </si>
   <si>
     <t>Bordereau d'envoi</t>
+  </si>
+  <si>
+    <t>le</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,16 +130,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>647699</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123303</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114064</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>237476</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353377</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>107373</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -152,7 +155,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -165,8 +168,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6195059" y="114064"/>
-          <a:ext cx="1174737" cy="876536"/>
+          <a:off x="123303" y="76201"/>
+          <a:ext cx="1023247" cy="765463"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -474,40 +477,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A7:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D1" s="1" t="s">
+    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F11" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G11" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>